<commit_message>
updated Tiang, Yalunka; fixed typo for Southern Ma'di
</commit_message>
<xml_diff>
--- a/raw/xlsx/numerals-sout2828-1.xlsx
+++ b/raw/xlsx/numerals-sout2828-1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bibiko/Documents/Developments/shh_git/numeralbank/numerals/raw/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65EE3EE7-67A9-344D-9803-CCEB3F637B81}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{464FF33E-57C6-B943-A3D6-2CDA46411B95}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="520" yWindow="460" windowWidth="28280" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="520" yWindow="460" windowWidth="28280" windowHeight="17540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -95,9 +95,6 @@
     <t>Madi-Southern.htm</t>
   </si>
   <si>
-    <t>quniary</t>
-  </si>
-  <si>
     <t>南部马迪语</t>
   </si>
   <si>
@@ -372,6 +369,9 @@
   </si>
   <si>
     <t>alɨ̀fʉ ìrì</t>
+  </si>
+  <si>
+    <t>quinary</t>
   </si>
 </sst>
 </file>
@@ -748,7 +748,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C42" sqref="C42"/>
     </sheetView>
@@ -779,467 +779,467 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:5" ht="31" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>32</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>33</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
     </row>
-    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:5" ht="31" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>34</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>35</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
     </row>
-    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:5" ht="31" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>36</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>37</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
     </row>
-    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:5" ht="31" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>38</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>39</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
     </row>
-    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:5" ht="31" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>40</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>41</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
     </row>
-    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:5" ht="31" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>42</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>43</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
     </row>
-    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:5" ht="31" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>44</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>45</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
     </row>
-    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:5" ht="31" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>46</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>47</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
     </row>
-    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:5" ht="31" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>48</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>49</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
     </row>
-    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:5" ht="31" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>50</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>51</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
     </row>
-    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:5" ht="31" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>52</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>53</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
     </row>
-    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:5" ht="31" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>54</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>55</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
     </row>
-    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:5" ht="31" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B14" s="3" t="s">
         <v>56</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>57</v>
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
     </row>
-    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:5" ht="31" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>58</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>59</v>
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
     </row>
-    <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:5" ht="31" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B16" s="3" t="s">
         <v>60</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>61</v>
       </c>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
     </row>
-    <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:5" ht="31" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B17" s="3" t="s">
         <v>62</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>63</v>
       </c>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
     </row>
-    <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:5" ht="31" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B18" s="3" t="s">
         <v>64</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>65</v>
       </c>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
     </row>
-    <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:5" ht="31" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B19" s="3" t="s">
         <v>66</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>67</v>
       </c>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
     </row>
-    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:5" ht="31" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B20" s="3" t="s">
         <v>68</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>69</v>
       </c>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
     </row>
-    <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:5" ht="31" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B21" s="3" t="s">
         <v>70</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>71</v>
       </c>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
     </row>
-    <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:5" ht="31" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B22" s="3" t="s">
         <v>72</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>73</v>
       </c>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
     </row>
-    <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:5" ht="31" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B23" s="3" t="s">
         <v>74</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>75</v>
       </c>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
     </row>
-    <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:5" ht="31" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B24" s="3" t="s">
         <v>76</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>77</v>
       </c>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
     </row>
-    <row r="25" spans="1:5" ht="30" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:5" ht="31" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B25" s="3" t="s">
         <v>78</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>79</v>
       </c>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
     </row>
-    <row r="26" spans="1:5" ht="30" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:5" ht="31" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B26" s="3" t="s">
         <v>80</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>81</v>
       </c>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
     </row>
-    <row r="27" spans="1:5" ht="30" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:5" ht="31" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B27" s="3" t="s">
         <v>82</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>83</v>
       </c>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
     </row>
-    <row r="28" spans="1:5" ht="30" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:5" ht="31" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B28" s="3" t="s">
         <v>84</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>85</v>
       </c>
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
     </row>
-    <row r="29" spans="1:5" ht="30" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:5" ht="31" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B29" s="3" t="s">
         <v>86</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>87</v>
       </c>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
       <c r="E29" s="3"/>
     </row>
-    <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:5" ht="31" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B30" s="3" t="s">
         <v>88</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>89</v>
       </c>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
     </row>
-    <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:5" ht="31" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B31" s="3" t="s">
         <v>90</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>91</v>
       </c>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
       <c r="E31" s="3"/>
     </row>
-    <row r="32" spans="1:5" ht="30" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:5" ht="31" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B32" s="3" t="s">
         <v>92</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>93</v>
       </c>
       <c r="C32" s="3"/>
       <c r="D32" s="3"/>
       <c r="E32" s="3"/>
     </row>
-    <row r="33" spans="1:5" ht="30" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:5" ht="31" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B33" s="3" t="s">
         <v>94</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>95</v>
       </c>
       <c r="C33" s="3"/>
       <c r="D33" s="3"/>
       <c r="E33" s="3"/>
     </row>
-    <row r="34" spans="1:5" ht="30" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:5" ht="31" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B34" s="3" t="s">
         <v>96</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>97</v>
       </c>
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
       <c r="E34" s="3"/>
     </row>
-    <row r="35" spans="1:5" ht="30" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:5" ht="31" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B35" s="3" t="s">
         <v>98</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>99</v>
       </c>
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
       <c r="E35" s="3"/>
     </row>
-    <row r="36" spans="1:5" ht="30" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:5" ht="31" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B36" s="3" t="s">
         <v>100</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>101</v>
       </c>
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
       <c r="E36" s="3"/>
     </row>
-    <row r="37" spans="1:5" ht="30" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:5" ht="31" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B37" s="3" t="s">
         <v>102</v>
-      </c>
-      <c r="B37" s="3" t="s">
-        <v>103</v>
       </c>
       <c r="C37" s="3"/>
       <c r="D37" s="3"/>
       <c r="E37" s="3"/>
     </row>
-    <row r="38" spans="1:5" ht="30" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:5" ht="31" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B38" s="3" t="s">
         <v>104</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>105</v>
       </c>
       <c r="C38" s="3"/>
       <c r="D38" s="3"/>
       <c r="E38" s="3"/>
     </row>
-    <row r="39" spans="1:5" ht="30" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:5" ht="31" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B39" s="3" t="s">
         <v>106</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>107</v>
       </c>
       <c r="C39" s="3"/>
       <c r="D39" s="3"/>
       <c r="E39" s="3"/>
     </row>
-    <row r="40" spans="1:5" ht="30" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:5" ht="31" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B40" s="3" t="s">
         <v>108</v>
-      </c>
-      <c r="B40" s="3" t="s">
-        <v>109</v>
       </c>
       <c r="C40" s="3"/>
       <c r="D40" s="3"/>
       <c r="E40" s="3"/>
     </row>
-    <row r="41" spans="1:5" ht="30" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:5" ht="31" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B41" s="3" t="s">
         <v>110</v>
-      </c>
-      <c r="B41" s="3" t="s">
-        <v>111</v>
       </c>
       <c r="C41" s="3"/>
       <c r="D41" s="3"/>
       <c r="E41" s="3"/>
     </row>
-    <row r="42" spans="1:5" ht="30" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:5" ht="31" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B42" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="B42" s="3" t="s">
+      <c r="C42" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="C42" s="3" t="s">
+      <c r="D42" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E42" s="3"/>
+    </row>
+    <row r="43" spans="1:5" ht="31" x14ac:dyDescent="0.55000000000000004">
+      <c r="A43" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="D42" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E42" s="3"/>
-    </row>
-    <row r="43" spans="1:5" ht="30" x14ac:dyDescent="0.55000000000000004">
-      <c r="A43" s="2" t="s">
+      <c r="B43" s="3" t="s">
         <v>115</v>
-      </c>
-      <c r="B43" s="3" t="s">
-        <v>116</v>
       </c>
       <c r="C43" s="3"/>
       <c r="D43" s="3"/>
@@ -1254,8 +1254,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1264,7 +1264,7 @@
     <col min="2" max="2" width="175" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="30" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" ht="31" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>5</v>
       </c>
@@ -1293,10 +1293,10 @@
         <v>8</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="30" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="31" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>9</v>
       </c>
@@ -1309,7 +1309,7 @@
         <v>10</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>24</v>
+        <v>116</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="31" x14ac:dyDescent="0.2">
@@ -1317,15 +1317,15 @@
         <v>11</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="30" x14ac:dyDescent="0.2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="31" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>12</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="31" x14ac:dyDescent="0.2">
@@ -1333,7 +1333,7 @@
         <v>13</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="30" x14ac:dyDescent="0.2">
@@ -1353,7 +1353,7 @@
         <v>16</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="31" x14ac:dyDescent="0.2">
@@ -1361,7 +1361,7 @@
         <v>17</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="30" x14ac:dyDescent="0.2">
@@ -1370,12 +1370,12 @@
       </c>
       <c r="B14" s="5"/>
     </row>
-    <row r="15" spans="1:2" ht="409.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>19</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>